<commit_message>
Se rellena de ejemplo, el excel
</commit_message>
<xml_diff>
--- a/gestion_proyecto/gestion-proyecto.xlsx
+++ b/gestion_proyecto/gestion-proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\tienda_online_fullstack_java\tienda-full-stack-java\gestion_proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raul\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09F2C26B-AECF-4EBF-813F-65CAF2BEDCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBC90E1-4FC7-441D-80D7-21D4DD0F0295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="0" windowWidth="18830" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iagrama de Gantt simple - BLANK" sheetId="2" r:id="rId1"/>
@@ -192,9 +192,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -931,11 +932,8 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1083,25 +1081,13 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,16 +1107,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1139,6 +1115,37 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,9 +1359,9 @@
   </sheetPr>
   <dimension ref="B1:W35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1368,67 +1375,67 @@
     <col min="9" max="23" width="3.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" s="24" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="2:23" s="23" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-    </row>
-    <row r="2" spans="2:23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="53" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+    </row>
+    <row r="2" spans="2:23" s="1" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:23" s="2" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="56" t="s">
+    <row r="3" spans="2:23" s="1" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:23" s="2" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55" t="s">
+    <row r="4" spans="2:23" s="1" customFormat="1" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:23" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="54" t="s">
+    <row r="5" spans="2:23" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="51"/>
-    </row>
-    <row r="6" spans="2:23" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="3"/>
+      <c r="C5" s="50"/>
+    </row>
+    <row r="6" spans="2:23" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="2:23" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="79" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="76" t="s">
         <v>4</v>
       </c>
       <c r="J7" s="77"/>
@@ -1447,742 +1454,802 @@
       <c r="W7" s="78"/>
     </row>
     <row r="8" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="76" t="s">
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="76" t="s">
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="75"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="80"/>
+      <c r="V8" s="80"/>
+      <c r="W8" s="81"/>
     </row>
     <row r="9" spans="2:23" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="S9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="14" t="s">
+      <c r="T9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="14" t="s">
+      <c r="U9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="V9" s="14" t="s">
+      <c r="V9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:23" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>1</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="30" t="str">
+      <c r="D10" s="28"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="29" t="str">
         <f t="shared" ref="G10:G28" si="0">IF(F10-E10=0,"",F10-E10)</f>
         <v/>
       </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="17"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="16"/>
     </row>
     <row r="11" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="68" t="str">
+      <c r="D11" s="32"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="47">
         <v>0</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="20"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="19"/>
     </row>
     <row r="12" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="68" t="str">
+      <c r="D12" s="34"/>
+      <c r="E12" s="83">
+        <v>44969</v>
+      </c>
+      <c r="F12" s="84">
+        <v>44969</v>
+      </c>
+      <c r="G12" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="47">
         <v>0</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="20"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="19"/>
     </row>
     <row r="13" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="31">
+      <c r="B13" s="30">
         <v>1.2</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="68" t="str">
+      <c r="D13" s="32"/>
+      <c r="E13" s="83">
+        <v>44969</v>
+      </c>
+      <c r="F13" s="84">
+        <v>44971</v>
+      </c>
+      <c r="G13" s="63">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="47">
+        <v>0</v>
+      </c>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="19"/>
+    </row>
+    <row r="14" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="30">
+        <v>1.3</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="83">
+        <v>44971</v>
+      </c>
+      <c r="F14" s="84">
+        <v>44971</v>
+      </c>
+      <c r="G14" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H13" s="48">
+      <c r="H14" s="47">
         <v>0</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="20"/>
-    </row>
-    <row r="14" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="31">
-        <v>1.3</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="68" t="str">
+      <c r="I14" s="42"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="19"/>
+    </row>
+    <row r="15" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="30">
+        <v>1.4</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="83">
+        <v>44971</v>
+      </c>
+      <c r="F15" s="84">
+        <v>44971</v>
+      </c>
+      <c r="G15" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H14" s="48">
+      <c r="H15" s="47">
         <v>0</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="20"/>
-    </row>
-    <row r="15" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="31">
-        <v>1.4</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="68" t="str">
+      <c r="I15" s="42"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="19"/>
+    </row>
+    <row r="16" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="83">
+        <v>44971</v>
+      </c>
+      <c r="F16" s="84">
+        <v>44973</v>
+      </c>
+      <c r="G16" s="63">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="47">
+        <v>0</v>
+      </c>
+      <c r="I16" s="42"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="19"/>
+    </row>
+    <row r="17" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="30">
+        <v>1.6</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="83">
+        <v>44973</v>
+      </c>
+      <c r="F17" s="84">
+        <v>44973</v>
+      </c>
+      <c r="G17" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H15" s="48">
+      <c r="H17" s="47">
         <v>0</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="20"/>
-    </row>
-    <row r="16" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="68" t="str">
+      <c r="I17" s="42"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="19"/>
+    </row>
+    <row r="18" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="30">
+        <v>2</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="37" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H16" s="48">
-        <v>0</v>
-      </c>
-      <c r="I16" s="43"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="20"/>
-    </row>
-    <row r="17" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="68" t="str">
+      <c r="H18" s="48"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="16"/>
+    </row>
+    <row r="19" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="30">
+        <v>2.1</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="83">
+        <v>44977</v>
+      </c>
+      <c r="F19" s="84">
+        <v>44977</v>
+      </c>
+      <c r="G19" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H17" s="48">
+      <c r="H19" s="47">
         <v>0</v>
       </c>
-      <c r="I17" s="43"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="20"/>
-    </row>
-    <row r="18" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="31">
-        <v>2</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="38" t="str">
+      <c r="I19" s="42"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="19"/>
+    </row>
+    <row r="20" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="83">
+        <v>44977</v>
+      </c>
+      <c r="F20" s="84">
+        <v>44977</v>
+      </c>
+      <c r="G20" s="63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="17"/>
-    </row>
-    <row r="19" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="31">
-        <v>2.1</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="68" t="str">
+      <c r="H20" s="47">
+        <v>0</v>
+      </c>
+      <c r="I20" s="42"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="19"/>
+    </row>
+    <row r="21" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="83">
+        <v>44978</v>
+      </c>
+      <c r="F21" s="84">
+        <v>44980</v>
+      </c>
+      <c r="G21" s="63">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="47">
+        <v>0</v>
+      </c>
+      <c r="I21" s="42"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="19"/>
+    </row>
+    <row r="22" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="30">
+        <v>2.4</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="83">
+        <v>44980</v>
+      </c>
+      <c r="F22" s="84">
+        <v>44981</v>
+      </c>
+      <c r="G22" s="63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="47">
+        <v>0</v>
+      </c>
+      <c r="I22" s="42"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="19"/>
+    </row>
+    <row r="23" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="30">
+        <v>3</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="37" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H19" s="48">
+      <c r="H23" s="48"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="16"/>
+    </row>
+    <row r="24" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="30">
+        <v>3.1</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="32"/>
+      <c r="E24" s="83">
+        <v>44970</v>
+      </c>
+      <c r="F24" s="84">
+        <v>44984</v>
+      </c>
+      <c r="G24" s="63">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H24" s="47">
         <v>0</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="20"/>
-    </row>
-    <row r="20" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="31">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="68" t="str">
+      <c r="I24" s="42"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="75"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="19"/>
+    </row>
+    <row r="25" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="30">
+        <v>3.2</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="83">
+        <v>44973</v>
+      </c>
+      <c r="F25" s="84">
+        <v>44985</v>
+      </c>
+      <c r="G25" s="63">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H20" s="48">
+        <v>12</v>
+      </c>
+      <c r="H25" s="47">
         <v>0</v>
       </c>
-      <c r="I20" s="43"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="20"/>
-    </row>
-    <row r="21" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="68" t="str">
+      <c r="I25" s="42"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="19"/>
+    </row>
+    <row r="26" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="34"/>
+      <c r="E26" s="83">
+        <v>44981</v>
+      </c>
+      <c r="F26" s="84">
+        <v>44987</v>
+      </c>
+      <c r="G26" s="63">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H21" s="48">
+        <v>6</v>
+      </c>
+      <c r="H26" s="47">
         <v>0</v>
       </c>
-      <c r="I21" s="43"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="20"/>
-    </row>
-    <row r="22" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="31">
-        <v>2.4</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="68" t="str">
+      <c r="I26" s="42"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="75"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="75"/>
+      <c r="W26" s="19"/>
+    </row>
+    <row r="27" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="83">
+        <v>44981</v>
+      </c>
+      <c r="F27" s="84">
+        <v>44987</v>
+      </c>
+      <c r="G27" s="63">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H22" s="48">
+        <v>6</v>
+      </c>
+      <c r="H27" s="47">
         <v>0</v>
       </c>
-      <c r="I22" s="43"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="85"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="20"/>
-    </row>
-    <row r="23" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="31">
-        <v>3</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="38" t="str">
+      <c r="I27" s="42"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="75"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V27" s="75"/>
+      <c r="W27" s="19"/>
+    </row>
+    <row r="28" spans="2:23" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="87">
+        <v>44987</v>
+      </c>
+      <c r="F28" s="88">
+        <v>44988</v>
+      </c>
+      <c r="G28" s="64">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H23" s="49"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="17"/>
-    </row>
-    <row r="24" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="31">
-        <v>3.1</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H24" s="48">
+        <v>1</v>
+      </c>
+      <c r="H28" s="49">
         <v>0</v>
       </c>
-      <c r="I24" s="43"/>
-      <c r="J24" s="86"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="86"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="20"/>
-    </row>
-    <row r="25" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="31">
-        <v>3.2</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H25" s="48">
-        <v>0</v>
-      </c>
-      <c r="I25" s="43"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="86"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="86"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="20"/>
-    </row>
-    <row r="26" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H26" s="48">
-        <v>0</v>
-      </c>
-      <c r="I26" s="43"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="86"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="86"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="20"/>
-    </row>
-    <row r="27" spans="2:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="68" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H27" s="48">
-        <v>0</v>
-      </c>
-      <c r="I27" s="43"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="86"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="V27" s="86"/>
-      <c r="W27" s="20"/>
-    </row>
-    <row r="28" spans="2:23" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="69" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H28" s="50">
-        <v>0</v>
-      </c>
-      <c r="I28" s="44"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="86"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="75"/>
     </row>
     <row r="35" spans="3:3" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="4"/>
+      <c r="C35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Nuevo cambio en excel
</commit_message>
<xml_diff>
--- a/gestion_proyecto/gestion-proyecto.xlsx
+++ b/gestion_proyecto/gestion-proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\tienda_online_fullstack_java\tienda-full-stack-java\gestion_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37428AC9-AA12-48FB-B8CB-141CD4BE421B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95530E72-5DA8-4A61-8287-3EE18DA963B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1358,7 +1358,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X25" sqref="X25"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2081,15 +2081,15 @@
       </c>
       <c r="I24" s="42"/>
       <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="17"/>
       <c r="T24" s="17"/>
       <c r="U24" s="17"/>
       <c r="V24" s="17"/>

</xml_diff>